<commit_message>
Updated database schema, uploaded resttt glitch code
</commit_message>
<xml_diff>
--- a/database schema.xlsx
+++ b/database schema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\git\vinhill.github.io\TTT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\git\TTTStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F3BF24-5031-4AE0-AF61-13F9A18909C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980B55FF-380E-43CE-80F8-3F23DC5031B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{999ED5BF-1C97-4366-969E-3A684A32F4E0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
   <si>
     <t>mid</t>
   </si>
@@ -41,9 +41,6 @@
     <t>map</t>
   </si>
   <si>
-    <t>result</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -56,12 +53,6 @@
     <t>TEXT</t>
   </si>
   <si>
-    <t>roles(team)</t>
-  </si>
-  <si>
-    <t>INTEGER</t>
-  </si>
-  <si>
     <t>ttt_troubleisland</t>
   </si>
   <si>
@@ -86,9 +77,6 @@
     <t>role</t>
   </si>
   <si>
-    <t>match(mid)</t>
-  </si>
-  <si>
     <t>player(name)</t>
   </si>
   <si>
@@ -104,9 +92,6 @@
     <t>roles</t>
   </si>
   <si>
-    <t>match</t>
-  </si>
-  <si>
     <t>Assassin</t>
   </si>
   <si>
@@ -159,6 +144,36 @@
   </si>
   <si>
     <t>#843001</t>
+  </si>
+  <si>
+    <t>round</t>
+  </si>
+  <si>
+    <t>ENUM</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>winner</t>
+  </si>
+  <si>
+    <t>VARCHAR(30)</t>
+  </si>
+  <si>
+    <t>round(mid)</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>configs</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>config.log</t>
   </si>
 </sst>
 </file>
@@ -399,6 +414,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -408,65 +429,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <font>
         <b/>
@@ -512,21 +479,24 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </top>
         <bottom style="medium">
           <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
     </dxf>
@@ -550,6 +520,30 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
@@ -591,11 +585,79 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -635,6 +697,49 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </top>
@@ -743,13 +848,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E1C6EE2-18C0-43EE-8AD5-4B7F873C290E}" name="Tabelle1" displayName="Tabelle1" ref="B3:F5" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E1C6EE2-18C0-43EE-8AD5-4B7F873C290E}" name="Tabelle1" displayName="Tabelle1" ref="B3:F5" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="B3:F5" xr:uid="{52BD7EF9-37E0-4ECA-A811-5669E3CF00AA}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{28B5F67C-42FE-4CC0-9F2B-12521EDBA32C}" name=" " dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{28B5F67C-42FE-4CC0-9F2B-12521EDBA32C}" name=" " dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{F6E5BE1F-762D-4412-BB71-B6D6EE94D6C5}" name="mid"/>
     <tableColumn id="3" xr3:uid="{820B8EBD-28D3-4E1A-8BDA-917DE40A720A}" name="map"/>
-    <tableColumn id="4" xr3:uid="{11082424-E386-4D0A-A5BC-F4137AB0998A}" name="result"/>
+    <tableColumn id="4" xr3:uid="{11082424-E386-4D0A-A5BC-F4137AB0998A}" name="winner"/>
     <tableColumn id="5" xr3:uid="{4DD32033-EEC8-40B7-B044-AC965EEDD732}" name="date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -757,10 +862,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC29E10A-9C08-4A05-9086-C9A760B6125F}" name="Tabelle2" displayName="Tabelle2" ref="H3:I5" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC29E10A-9C08-4A05-9086-C9A760B6125F}" name="Tabelle2" displayName="Tabelle2" ref="H3:I5" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="H3:I5" xr:uid="{454A1DA6-4CBA-4EE8-9389-936CF1CDD9C1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{239B428F-5914-4616-BB28-ACE39A22434A}" name=" " dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{239B428F-5914-4616-BB28-ACE39A22434A}" name=" " dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{907C80F7-F928-48C1-B45D-8B7F2BD81756}" name="name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -768,10 +873,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7C718E60-F6FD-436B-A6CB-DA9764FFB495}" name="Tabelle3" displayName="Tabelle3" ref="B8:E10" totalsRowShown="0" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7C718E60-F6FD-436B-A6CB-DA9764FFB495}" name="Tabelle3" displayName="Tabelle3" ref="B8:E10" totalsRowShown="0" tableBorderDxfId="13">
   <autoFilter ref="B8:E10" xr:uid="{BAA7DE8C-DD5A-4893-B04B-F30191F23A0B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{44C27546-60CC-4084-8DA7-938121BD4DD8}" name=" " dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{44C27546-60CC-4084-8DA7-938121BD4DD8}" name=" " dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{F875BBA2-5C66-4170-A8BA-302DED26D730}" name="mid"/>
     <tableColumn id="3" xr3:uid="{B1CBFB62-9386-4E51-BA90-66DF49A5C99C}" name="player"/>
     <tableColumn id="4" xr3:uid="{D89E7C9A-4FB1-41B5-AB65-25E7E69B1C82}" name="role"/>
@@ -781,10 +886,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{822FCC4F-55FE-41D3-B688-A3BC9AB95087}" name="Tabelle4" displayName="Tabelle4" ref="G8:J10" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{822FCC4F-55FE-41D3-B688-A3BC9AB95087}" name="Tabelle4" displayName="Tabelle4" ref="G8:J10" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="G8:J10" xr:uid="{F52E8E40-021E-4471-BC10-A9FF1FC8BA38}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5A1BBBC7-2810-44CB-B915-737D559B2C6D}" name=" " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{5A1BBBC7-2810-44CB-B915-737D559B2C6D}" name=" " dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{75A0585B-E744-4BCE-9B14-593A7F63D81D}" name="role"/>
     <tableColumn id="3" xr3:uid="{0C542851-5D2F-4808-AFF8-3C2F0C30C757}" name="team"/>
     <tableColumn id="4" xr3:uid="{8B4D4879-D6B4-439F-B598-56E784F06DFD}" name="colour"/>
@@ -797,7 +902,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{357D6CAA-DF33-46C1-8889-58556704D715}" name="Tabelle5" displayName="Tabelle5" ref="B13:H15" totalsRowShown="0">
   <autoFilter ref="B13:H15" xr:uid="{32C5A8BE-07D8-4186-A1ED-263E5296B241}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0CE5F855-0B92-46E6-921D-AB0B2AC4DB13}" name=" " dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{0CE5F855-0B92-46E6-921D-AB0B2AC4DB13}" name=" " dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{A3F198A1-4906-4DB2-A4FC-D49EAEF17788}" name="mid"/>
     <tableColumn id="3" xr3:uid="{1F3F8CE0-77E8-449C-85EA-DFB6C4FC4937}" name="attacker"/>
     <tableColumn id="4" xr3:uid="{7A6DF6C9-10C2-4CB8-A498-83737D30FD4B}" name="victim"/>
@@ -813,7 +918,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2FF55995-BED1-4ADB-8024-4F3E431A361D}" name="Tabelle57" displayName="Tabelle57" ref="B18:I20" totalsRowShown="0">
   <autoFilter ref="B18:I20" xr:uid="{401E65C2-71AC-4B06-B98F-F12946593E95}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A71BEE10-E42F-432F-981C-A4CE4BA19270}" name=" " dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{A71BEE10-E42F-432F-981C-A4CE4BA19270}" name=" " dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{0418B8D0-A27E-45B4-95A3-7A28A7873426}" name="mid"/>
     <tableColumn id="3" xr3:uid="{57C7490B-1122-431F-83F9-91FE827D5B21}" name="attacker"/>
     <tableColumn id="4" xr3:uid="{3C2AB111-3F7D-4D50-9026-C3030824B528}" name="victim"/>
@@ -821,6 +926,17 @@
     <tableColumn id="6" xr3:uid="{9AC775AF-AC84-4C13-BF45-5B4A0C62973D}" name="vktrol"/>
     <tableColumn id="7" xr3:uid="{1AE8D86E-4139-4F82-A700-C24D560F70B3}" name="time"/>
     <tableColumn id="8" xr3:uid="{810AC511-47D1-47A2-80EB-E6D1478028FC}" name="damage"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C1563867-70DF-4091-83F3-B3B42F5161BB}" name="Tabelle28" displayName="Tabelle28" ref="B23:C25" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3" totalsRowBorderDxfId="1">
+  <autoFilter ref="B23:C25" xr:uid="{11560C94-C78A-4C22-B229-87B96A147E98}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{847738E0-6F98-4A70-A98A-2FB31829D010}" name=" " dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{066970CC-1FA8-43B1-9EC6-AE9D55C6A3F3}" name="filename"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1126,42 +1242,42 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J20"/>
+  <dimension ref="B1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J20"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23"/>
-      <c r="H2" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="23"/>
+      <c r="B2" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
+      <c r="H2" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>0</v>
@@ -1170,331 +1286,363 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="H3" s="17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="9">
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F5" s="10">
         <v>44342</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
-      <c r="G7" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="26"/>
+      <c r="B7" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="G7" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="28" t="s">
-        <v>40</v>
+        <v>13</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>38</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="15">
         <v>1</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="29" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>7</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="23"/>
+      <c r="B12" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="29"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="9">
         <v>1</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="23"/>
+      <c r="B17" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="29"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="9">
         <v>1</v>
       </c>
       <c r="D20" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="I20" s="20">
         <v>40</v>
       </c>
     </row>
+    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="29"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B12:H12"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B2:F2"/>
@@ -1504,13 +1652,14 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId1"/>
-  <tableParts count="6">
+  <tableParts count="7">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update db table schema
</commit_message>
<xml_diff>
--- a/database schema.xlsx
+++ b/database schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\git\TTTStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980B55FF-380E-43CE-80F8-3F23DC5031B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BA5A9F-F574-40C6-89B8-71BF3A003B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{999ED5BF-1C97-4366-969E-3A684A32F4E0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{999ED5BF-1C97-4366-969E-3A684A32F4E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="67">
   <si>
     <t>mid</t>
   </si>
@@ -50,15 +50,9 @@
     <t>Example</t>
   </si>
   <si>
-    <t>TEXT</t>
-  </si>
-  <si>
     <t>ttt_troubleisland</t>
   </si>
   <si>
-    <t>Traitors</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -80,45 +74,21 @@
     <t>player(name)</t>
   </si>
   <si>
-    <t>roles(role)</t>
-  </si>
-  <si>
     <t>Poci</t>
   </si>
   <si>
     <t>Traitor</t>
   </si>
   <si>
-    <t>roles</t>
-  </si>
-  <si>
-    <t>Assassin</t>
-  </si>
-  <si>
-    <t>kills</t>
-  </si>
-  <si>
-    <t>attacker</t>
-  </si>
-  <si>
-    <t>victim</t>
-  </si>
-  <si>
     <t>atkrole</t>
   </si>
   <si>
-    <t>vktrol</t>
-  </si>
-  <si>
     <t>time</t>
   </si>
   <si>
     <t>Schnitzelboy</t>
   </si>
   <si>
-    <t>GhastM4n</t>
-  </si>
-  <si>
     <t>01:32.62</t>
   </si>
   <si>
@@ -128,36 +98,24 @@
     <t>damage</t>
   </si>
   <si>
-    <t>01:30.69</t>
-  </si>
-  <si>
     <t>vktrole</t>
   </si>
   <si>
     <t>team</t>
   </si>
   <si>
-    <t>Mercenary</t>
-  </si>
-  <si>
     <t>colour</t>
   </si>
   <si>
     <t>#843001</t>
   </si>
   <si>
-    <t>round</t>
-  </si>
-  <si>
     <t>ENUM</t>
   </si>
   <si>
     <t>INT</t>
   </si>
   <si>
-    <t>winner</t>
-  </si>
-  <si>
     <t>VARCHAR(30)</t>
   </si>
   <si>
@@ -174,6 +132,108 @@
   </si>
   <si>
     <t>config.log</t>
+  </si>
+  <si>
+    <t>match</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>superteam</t>
+  </si>
+  <si>
+    <t>Necromancer</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>startrole</t>
+  </si>
+  <si>
+    <t>mainrole</t>
+  </si>
+  <si>
+    <t>role(name)</t>
+  </si>
+  <si>
+    <t>Drunk</t>
+  </si>
+  <si>
+    <t>match(mid)</t>
+  </si>
+  <si>
+    <t>wins</t>
+  </si>
+  <si>
+    <t>role(team)</t>
+  </si>
+  <si>
+    <t>Innocent</t>
+  </si>
+  <si>
+    <t>loves</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>dies</t>
+  </si>
+  <si>
+    <t>revives</t>
+  </si>
+  <si>
+    <t>rolechange</t>
+  </si>
+  <si>
+    <t>buys</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>causee</t>
+  </si>
+  <si>
+    <t>fromrole</t>
+  </si>
+  <si>
+    <t>torole</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>weapon</t>
+  </si>
+  <si>
+    <t>fight</t>
+  </si>
+  <si>
+    <t>fall</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>04:32.1</t>
+  </si>
+  <si>
+    <t>Ghastman</t>
+  </si>
+  <si>
+    <t>Crowbar</t>
+  </si>
+  <si>
+    <t>V8Block</t>
   </si>
 </sst>
 </file>
@@ -234,7 +294,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -388,11 +448,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -416,24 +513,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="30">
     <dxf>
       <font>
         <b/>
@@ -471,16 +579,39 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <bottom style="medium">
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
@@ -492,9 +623,32 @@
         <right style="medium">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
@@ -520,30 +674,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
@@ -585,30 +715,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -617,9 +723,19 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </top>
@@ -627,37 +743,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -696,11 +781,52 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-      </border>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -793,6 +919,64 @@
       </fill>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -815,6 +999,72 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -848,24 +1098,66 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E1C6EE2-18C0-43EE-8AD5-4B7F873C290E}" name="Tabelle1" displayName="Tabelle1" ref="B3:F5" totalsRowShown="0" headerRowDxfId="20">
-  <autoFilter ref="B3:F5" xr:uid="{52BD7EF9-37E0-4ECA-A811-5669E3CF00AA}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{28B5F67C-42FE-4CC0-9F2B-12521EDBA32C}" name=" " dataDxfId="19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E1C6EE2-18C0-43EE-8AD5-4B7F873C290E}" name="Tabelle1" displayName="Tabelle1" ref="B3:E5" totalsRowShown="0" headerRowDxfId="29">
+  <autoFilter ref="B3:E5" xr:uid="{52BD7EF9-37E0-4ECA-A811-5669E3CF00AA}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{28B5F67C-42FE-4CC0-9F2B-12521EDBA32C}" name=" " dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{F6E5BE1F-762D-4412-BB71-B6D6EE94D6C5}" name="mid"/>
     <tableColumn id="3" xr3:uid="{820B8EBD-28D3-4E1A-8BDA-917DE40A720A}" name="map"/>
-    <tableColumn id="4" xr3:uid="{11082424-E386-4D0A-A5BC-F4137AB0998A}" name="winner"/>
     <tableColumn id="5" xr3:uid="{4DD32033-EEC8-40B7-B044-AC965EEDD732}" name="date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{74C74E02-A02B-41C4-BADC-5A81D4707866}" name="Tabelle12" displayName="Tabelle12" ref="B23:H25" totalsRowShown="0" tableBorderDxfId="4">
+  <autoFilter ref="B23:H25" xr:uid="{74C74E02-A02B-41C4-BADC-5A81D4707866}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{2F3D3C50-1B81-4C2A-AC27-145F73A517B4}" name=" "/>
+    <tableColumn id="2" xr3:uid="{BFBE01E6-D2F9-4FEC-98E5-6FD7BFEE4A15}" name="mid"/>
+    <tableColumn id="3" xr3:uid="{D252F81D-FEAA-49CD-8D7B-FD6F074A08A2}" name="player"/>
+    <tableColumn id="4" xr3:uid="{8731F0A4-8107-43FD-9F22-FA4CF46A2C14}" name="causee"/>
+    <tableColumn id="5" xr3:uid="{6DFDAEE0-AEC1-45E5-9E8B-AA9DD78D8CBF}" name="fromrole"/>
+    <tableColumn id="6" xr3:uid="{398BB72D-970E-4531-9612-81F2C3C547E0}" name="torole"/>
+    <tableColumn id="7" xr3:uid="{D216005C-1E93-4949-AA8B-09D52C12C24A}" name="time"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{C6772C9E-B684-4967-B1B0-2F5D7E931EAD}" name="Tabelle13" displayName="Tabelle13" ref="L18:O20" totalsRowShown="0" tableBorderDxfId="3">
+  <autoFilter ref="L18:O20" xr:uid="{C6772C9E-B684-4967-B1B0-2F5D7E931EAD}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{11ADBF08-FA1E-4F08-91A9-89729F535445}" name=" "/>
+    <tableColumn id="2" xr3:uid="{754DA27A-3AA8-4E40-949D-9264EF980EDD}" name="mid"/>
+    <tableColumn id="3" xr3:uid="{6B3182E9-F4BF-4CA5-B320-DB44C252EF32}" name="first"/>
+    <tableColumn id="4" xr3:uid="{B089E9C9-3B3E-4AAF-9B5A-7F3033018EBB}" name="second"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B264D01E-B1C5-44AC-A123-09E78C0A1D3C}" name="Tabelle14" displayName="Tabelle14" ref="B13:F15" totalsRowShown="0" tableBorderDxfId="2">
+  <autoFilter ref="B13:F15" xr:uid="{B264D01E-B1C5-44AC-A123-09E78C0A1D3C}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{35CAF910-5E11-4C98-BDCB-833CA7FD7C95}" name=" "/>
+    <tableColumn id="2" xr3:uid="{71459494-1BA9-4A53-9244-FF1A5ADDCF75}" name="mid"/>
+    <tableColumn id="3" xr3:uid="{44814302-0FAB-4B5B-9D64-6AFE4783B793}" name="player"/>
+    <tableColumn id="4" xr3:uid="{F8AB16FD-080F-489A-9596-AF0E16856803}" name="item"/>
+    <tableColumn id="5" xr3:uid="{0AFE03ED-82E8-4D41-87C5-80B654E288B0}" name="time"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC29E10A-9C08-4A05-9086-C9A760B6125F}" name="Tabelle2" displayName="Tabelle2" ref="H3:I5" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
-  <autoFilter ref="H3:I5" xr:uid="{454A1DA6-4CBA-4EE8-9389-936CF1CDD9C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC29E10A-9C08-4A05-9086-C9A760B6125F}" name="Tabelle2" displayName="Tabelle2" ref="G3:H5" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+  <autoFilter ref="G3:H5" xr:uid="{454A1DA6-4CBA-4EE8-9389-936CF1CDD9C1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{239B428F-5914-4616-BB28-ACE39A22434A}" name=" " dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{239B428F-5914-4616-BB28-ACE39A22434A}" name=" " dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{907C80F7-F928-48C1-B45D-8B7F2BD81756}" name="name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -873,25 +1165,27 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7C718E60-F6FD-436B-A6CB-DA9764FFB495}" name="Tabelle3" displayName="Tabelle3" ref="B8:E10" totalsRowShown="0" tableBorderDxfId="13">
-  <autoFilter ref="B8:E10" xr:uid="{BAA7DE8C-DD5A-4893-B04B-F30191F23A0B}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{44C27546-60CC-4084-8DA7-938121BD4DD8}" name=" " dataDxfId="12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7C718E60-F6FD-436B-A6CB-DA9764FFB495}" name="Tabelle3" displayName="Tabelle3" ref="F18:J20" totalsRowShown="0" tableBorderDxfId="23">
+  <autoFilter ref="F18:J20" xr:uid="{BAA7DE8C-DD5A-4893-B04B-F30191F23A0B}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{44C27546-60CC-4084-8DA7-938121BD4DD8}" name=" " dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{F875BBA2-5C66-4170-A8BA-302DED26D730}" name="mid"/>
     <tableColumn id="3" xr3:uid="{B1CBFB62-9386-4E51-BA90-66DF49A5C99C}" name="player"/>
-    <tableColumn id="4" xr3:uid="{D89E7C9A-4FB1-41B5-AB65-25E7E69B1C82}" name="role"/>
+    <tableColumn id="5" xr3:uid="{8064CD73-A5FF-4E2A-94B3-03654FA70CCF}" name="startrole"/>
+    <tableColumn id="4" xr3:uid="{D89E7C9A-4FB1-41B5-AB65-25E7E69B1C82}" name="mainrole"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{822FCC4F-55FE-41D3-B688-A3BC9AB95087}" name="Tabelle4" displayName="Tabelle4" ref="G8:J10" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="G8:J10" xr:uid="{F52E8E40-021E-4471-BC10-A9FF1FC8BA38}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5A1BBBC7-2810-44CB-B915-737D559B2C6D}" name=" " dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{75A0585B-E744-4BCE-9B14-593A7F63D81D}" name="role"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{822FCC4F-55FE-41D3-B688-A3BC9AB95087}" name="Tabelle4" displayName="Tabelle4" ref="J3:N5" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+  <autoFilter ref="J3:N5" xr:uid="{F52E8E40-021E-4471-BC10-A9FF1FC8BA38}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{5A1BBBC7-2810-44CB-B915-737D559B2C6D}" name=" " dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{75A0585B-E744-4BCE-9B14-593A7F63D81D}" name="name"/>
     <tableColumn id="3" xr3:uid="{0C542851-5D2F-4808-AFF8-3C2F0C30C757}" name="team"/>
+    <tableColumn id="5" xr3:uid="{E1976BC6-4987-4D27-A165-640DCAC50A88}" name="superteam"/>
     <tableColumn id="4" xr3:uid="{8B4D4879-D6B4-439F-B598-56E784F06DFD}" name="colour"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -899,15 +1193,17 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{357D6CAA-DF33-46C1-8889-58556704D715}" name="Tabelle5" displayName="Tabelle5" ref="B13:H15" totalsRowShown="0">
-  <autoFilter ref="B13:H15" xr:uid="{32C5A8BE-07D8-4186-A1ED-263E5296B241}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0CE5F855-0B92-46E6-921D-AB0B2AC4DB13}" name=" " dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{357D6CAA-DF33-46C1-8889-58556704D715}" name="Tabelle5" displayName="Tabelle5" ref="H8:P10" totalsRowShown="0">
+  <autoFilter ref="H8:P10" xr:uid="{32C5A8BE-07D8-4186-A1ED-263E5296B241}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{0CE5F855-0B92-46E6-921D-AB0B2AC4DB13}" name=" " dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{A3F198A1-4906-4DB2-A4FC-D49EAEF17788}" name="mid"/>
-    <tableColumn id="3" xr3:uid="{1F3F8CE0-77E8-449C-85EA-DFB6C4FC4937}" name="attacker"/>
-    <tableColumn id="4" xr3:uid="{7A6DF6C9-10C2-4CB8-A498-83737D30FD4B}" name="victim"/>
-    <tableColumn id="5" xr3:uid="{664DF83E-1949-4D59-92CB-749EE758FC51}" name="atkrole"/>
-    <tableColumn id="6" xr3:uid="{7FA1D689-94F5-462A-9EEE-89397321EC4C}" name="vktrole"/>
+    <tableColumn id="3" xr3:uid="{1F3F8CE0-77E8-449C-85EA-DFB6C4FC4937}" name="player"/>
+    <tableColumn id="4" xr3:uid="{7A6DF6C9-10C2-4CB8-A498-83737D30FD4B}" name="vktrole"/>
+    <tableColumn id="5" xr3:uid="{664DF83E-1949-4D59-92CB-749EE758FC51}" name="reason"/>
+    <tableColumn id="6" xr3:uid="{7FA1D689-94F5-462A-9EEE-89397321EC4C}" name="causee"/>
+    <tableColumn id="9" xr3:uid="{4BEC3DB9-57AF-4B72-BB20-2A526C6A0ED9}" name="atkrole"/>
+    <tableColumn id="8" xr3:uid="{6B455A4E-61C8-4F7F-B6A4-252B2CB182F4}" name="weapon"/>
     <tableColumn id="7" xr3:uid="{6A5B3ED8-A41F-46F2-9BFB-DB1F20464E8A}" name="time"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -915,28 +1211,56 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2FF55995-BED1-4ADB-8024-4F3E431A361D}" name="Tabelle57" displayName="Tabelle57" ref="B18:I20" totalsRowShown="0">
-  <autoFilter ref="B18:I20" xr:uid="{401E65C2-71AC-4B06-B98F-F12946593E95}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A71BEE10-E42F-432F-981C-A4CE4BA19270}" name=" " dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2FF55995-BED1-4ADB-8024-4F3E431A361D}" name="Tabelle57" displayName="Tabelle57" ref="H13:Q15" totalsRowShown="0">
+  <autoFilter ref="H13:Q15" xr:uid="{401E65C2-71AC-4B06-B98F-F12946593E95}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{A71BEE10-E42F-432F-981C-A4CE4BA19270}" name=" " dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{0418B8D0-A27E-45B4-95A3-7A28A7873426}" name="mid"/>
-    <tableColumn id="3" xr3:uid="{57C7490B-1122-431F-83F9-91FE827D5B21}" name="attacker"/>
-    <tableColumn id="4" xr3:uid="{3C2AB111-3F7D-4D50-9026-C3030824B528}" name="victim"/>
-    <tableColumn id="5" xr3:uid="{62B85A24-0C98-4BB2-93AF-7415AEC1D177}" name="atkrole"/>
-    <tableColumn id="6" xr3:uid="{9AC775AF-AC84-4C13-BF45-5B4A0C62973D}" name="vktrol"/>
-    <tableColumn id="7" xr3:uid="{1AE8D86E-4139-4F82-A700-C24D560F70B3}" name="time"/>
-    <tableColumn id="8" xr3:uid="{810AC511-47D1-47A2-80EB-E6D1478028FC}" name="damage"/>
+    <tableColumn id="3" xr3:uid="{57C7490B-1122-431F-83F9-91FE827D5B21}" name="player"/>
+    <tableColumn id="4" xr3:uid="{3C2AB111-3F7D-4D50-9026-C3030824B528}" name="vktrole"/>
+    <tableColumn id="5" xr3:uid="{62B85A24-0C98-4BB2-93AF-7415AEC1D177}" name="reason"/>
+    <tableColumn id="6" xr3:uid="{9AC775AF-AC84-4C13-BF45-5B4A0C62973D}" name="causee"/>
+    <tableColumn id="7" xr3:uid="{1AE8D86E-4139-4F82-A700-C24D560F70B3}" name="atkrole"/>
+    <tableColumn id="10" xr3:uid="{FF555FE5-B1A8-402F-96B8-1915C15BDF86}" name="weapon"/>
+    <tableColumn id="9" xr3:uid="{6EA4795D-0357-4C1B-8960-A01B91FE8EBE}" name="damage"/>
+    <tableColumn id="8" xr3:uid="{810AC511-47D1-47A2-80EB-E6D1478028FC}" name="time"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C1563867-70DF-4091-83F3-B3B42F5161BB}" name="Tabelle28" displayName="Tabelle28" ref="B23:C25" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3" totalsRowBorderDxfId="1">
-  <autoFilter ref="B23:C25" xr:uid="{11560C94-C78A-4C22-B229-87B96A147E98}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C1563867-70DF-4091-83F3-B3B42F5161BB}" name="Tabelle28" displayName="Tabelle28" ref="P3:Q5" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+  <autoFilter ref="P3:Q5" xr:uid="{11560C94-C78A-4C22-B229-87B96A147E98}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{847738E0-6F98-4A70-A98A-2FB31829D010}" name=" " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{847738E0-6F98-4A70-A98A-2FB31829D010}" name=" " dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{066970CC-1FA8-43B1-9EC6-AE9D55C6A3F3}" name="filename"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C2022558-BCF4-4A20-A751-B2D365242E58}" name="Tabelle9" displayName="Tabelle9" ref="B18:D20" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <autoFilter ref="B18:D20" xr:uid="{C2022558-BCF4-4A20-A751-B2D365242E58}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{CF878C07-E058-4CC5-B0B0-D4A3103C0C4E}" name=" " dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{A74A4B78-31DD-4C7D-95C0-7D427DEA6813}" name="mid"/>
+    <tableColumn id="3" xr3:uid="{41CA0520-4406-4BF2-891F-364ED422B165}" name="team"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EB9ED773-AC33-429C-A78F-BDB6B255A40A}" name="Tabelle11" displayName="Tabelle11" ref="B8:F10" totalsRowShown="0" tableBorderDxfId="5">
+  <autoFilter ref="B8:F10" xr:uid="{EB9ED773-AC33-429C-A78F-BDB6B255A40A}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{FE18D11D-1881-4A20-81B1-CE46DB24D346}" name=" "/>
+    <tableColumn id="2" xr3:uid="{BF946692-53EE-4E40-94C7-D9CAD1117515}" name="mid"/>
+    <tableColumn id="3" xr3:uid="{08B630E2-F9B0-4E9C-A159-ECD4C24858E8}" name="player"/>
+    <tableColumn id="4" xr3:uid="{579BCD9B-7012-4A04-8008-E15E0C63293F}" name="causee"/>
+    <tableColumn id="5" xr3:uid="{75098097-761B-4423-8FDB-9C45E9EEF3BC}" name="reason"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1242,42 +1566,56 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J25"/>
+  <dimension ref="B1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
-        <v>37</v>
+    <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B2" s="26" t="s">
+        <v>33</v>
       </c>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
-      <c r="H2" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="29"/>
+      <c r="E2" s="27"/>
+      <c r="G2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="27"/>
+      <c r="J2" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="27"/>
+      <c r="P2" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="27"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>0</v>
@@ -1285,43 +1623,79 @@
       <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="G3" s="17" t="s">
+        <v>9</v>
+      </c>
       <c r="H3" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>41</v>
+      <c r="H4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
@@ -1329,330 +1703,567 @@
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="10">
+        <v>44342</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="10">
-        <v>44342</v>
-      </c>
-      <c r="H5" s="18" t="s">
+      <c r="J5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="19" t="s">
-        <v>9</v>
+      <c r="K5" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="27" t="s">
-        <v>10</v>
+    <row r="6" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="26" t="s">
+        <v>50</v>
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
-      <c r="G7" s="27" t="s">
+      <c r="E7" s="28"/>
+      <c r="F7" s="27"/>
+      <c r="H7" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="27"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="H10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="9">
+        <v>1</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="P10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="23"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="15">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="27" t="s">
-        <v>20</v>
+    <row r="11" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="26" t="s">
+        <v>52</v>
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
       <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="29"/>
+      <c r="F12" s="27"/>
+      <c r="H12" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="27"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
-        <v>11</v>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="7" t="s">
+      <c r="L13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="M14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q14" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>43</v>
+    <row r="15" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="H15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="9">
+        <v>1</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N15" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="O15" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="P15" s="9">
+        <v>10</v>
+      </c>
+      <c r="Q15" s="20" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="9">
-        <v>1</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
+    <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
+      <c r="F17" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
-      <c r="I17" s="29"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="27"/>
+      <c r="L17" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="27"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="6" t="s">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="D18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>24</v>
+      <c r="F18" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>0</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L19" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="19">
+        <v>1</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="15">
+        <v>1</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="J20" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="6" t="s">
+      <c r="L20" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" s="9">
+        <v>1</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="O20" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="27"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>39</v>
+      <c r="D24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="8" t="s">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C25" s="6">
         <v>1</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I20" s="20">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="29"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>46</v>
-      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="G7:I7"/>
+  <mergeCells count="12">
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="H12:Q12"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="H7:P7"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId1"/>
-  <tableParts count="7">
+  <pageSetup paperSize="9" scale="63" orientation="landscape" r:id="rId1"/>
+  <tableParts count="12">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -1660,6 +2271,11 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
script for cleaning logs
</commit_message>
<xml_diff>
--- a/database schema.xlsx
+++ b/database schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\git\TTTStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BA5A9F-F574-40C6-89B8-71BF3A003B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2831CEE-BCEE-4B7E-9277-4DA2FDA777D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{999ED5BF-1C97-4366-969E-3A684A32F4E0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="70">
   <si>
     <t>mid</t>
   </si>
@@ -134,9 +134,6 @@
     <t>config.log</t>
   </si>
   <si>
-    <t>match</t>
-  </si>
-  <si>
     <t>VARCHAR</t>
   </si>
   <si>
@@ -234,6 +231,18 @@
   </si>
   <si>
     <t>V8Block</t>
+  </si>
+  <si>
+    <t>game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>crole</t>
   </si>
 </sst>
 </file>
@@ -489,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -500,7 +509,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -516,18 +524,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -537,11 +544,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="34">
     <dxf>
       <font>
         <b/>
@@ -601,82 +609,18 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <bottom style="medium">
-          <color indexed="64"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -715,36 +659,6 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -805,28 +719,56 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -919,64 +861,6 @@
       </fill>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1078,6 +962,274 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -1098,39 +1250,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E1C6EE2-18C0-43EE-8AD5-4B7F873C290E}" name="Tabelle1" displayName="Tabelle1" ref="B3:E5" totalsRowShown="0" headerRowDxfId="29">
-  <autoFilter ref="B3:E5" xr:uid="{52BD7EF9-37E0-4ECA-A811-5669E3CF00AA}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{28B5F67C-42FE-4CC0-9F2B-12521EDBA32C}" name=" " dataDxfId="13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E1C6EE2-18C0-43EE-8AD5-4B7F873C290E}" name="Tabelle1" displayName="Tabelle1" ref="B3:F5" totalsRowShown="0" headerRowDxfId="33">
+  <autoFilter ref="B3:F5" xr:uid="{52BD7EF9-37E0-4ECA-A811-5669E3CF00AA}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{28B5F67C-42FE-4CC0-9F2B-12521EDBA32C}" name=" " dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{F6E5BE1F-762D-4412-BB71-B6D6EE94D6C5}" name="mid"/>
     <tableColumn id="3" xr3:uid="{820B8EBD-28D3-4E1A-8BDA-917DE40A720A}" name="map"/>
     <tableColumn id="5" xr3:uid="{4DD32033-EEC8-40B7-B044-AC965EEDD732}" name="date"/>
+    <tableColumn id="4" xr3:uid="{5F61BB11-1584-4F62-B16B-BAA250589FF5}" name="duration"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{74C74E02-A02B-41C4-BADC-5A81D4707866}" name="Tabelle12" displayName="Tabelle12" ref="B23:H25" totalsRowShown="0" tableBorderDxfId="4">
-  <autoFilter ref="B23:H25" xr:uid="{74C74E02-A02B-41C4-BADC-5A81D4707866}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2F3D3C50-1B81-4C2A-AC27-145F73A517B4}" name=" "/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{74C74E02-A02B-41C4-BADC-5A81D4707866}" name="Tabelle12" displayName="Tabelle12" ref="B23:I25" totalsRowShown="0" tableBorderDxfId="7">
+  <autoFilter ref="B23:I25" xr:uid="{74C74E02-A02B-41C4-BADC-5A81D4707866}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{2F3D3C50-1B81-4C2A-AC27-145F73A517B4}" name=" " dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{BFBE01E6-D2F9-4FEC-98E5-6FD7BFEE4A15}" name="mid"/>
     <tableColumn id="3" xr3:uid="{D252F81D-FEAA-49CD-8D7B-FD6F074A08A2}" name="player"/>
     <tableColumn id="4" xr3:uid="{8731F0A4-8107-43FD-9F22-FA4CF46A2C14}" name="causee"/>
     <tableColumn id="5" xr3:uid="{6DFDAEE0-AEC1-45E5-9E8B-AA9DD78D8CBF}" name="fromrole"/>
     <tableColumn id="6" xr3:uid="{398BB72D-970E-4531-9612-81F2C3C547E0}" name="torole"/>
     <tableColumn id="7" xr3:uid="{D216005C-1E93-4949-AA8B-09D52C12C24A}" name="time"/>
+    <tableColumn id="8" xr3:uid="{4F52CAD3-EA0D-4037-AE32-B99C8E0B1EA7}" name="crole"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{C6772C9E-B684-4967-B1B0-2F5D7E931EAD}" name="Tabelle13" displayName="Tabelle13" ref="L18:O20" totalsRowShown="0" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{C6772C9E-B684-4967-B1B0-2F5D7E931EAD}" name="Tabelle13" displayName="Tabelle13" ref="L18:O20" totalsRowShown="0" tableBorderDxfId="6">
   <autoFilter ref="L18:O20" xr:uid="{C6772C9E-B684-4967-B1B0-2F5D7E931EAD}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{11ADBF08-FA1E-4F08-91A9-89729F535445}" name=" "/>
+    <tableColumn id="1" xr3:uid="{11ADBF08-FA1E-4F08-91A9-89729F535445}" name=" " dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{754DA27A-3AA8-4E40-949D-9264EF980EDD}" name="mid"/>
     <tableColumn id="3" xr3:uid="{6B3182E9-F4BF-4CA5-B320-DB44C252EF32}" name="first"/>
     <tableColumn id="4" xr3:uid="{B089E9C9-3B3E-4AAF-9B5A-7F3033018EBB}" name="second"/>
@@ -1140,10 +1294,10 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B264D01E-B1C5-44AC-A123-09E78C0A1D3C}" name="Tabelle14" displayName="Tabelle14" ref="B13:F15" totalsRowShown="0" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B264D01E-B1C5-44AC-A123-09E78C0A1D3C}" name="Tabelle14" displayName="Tabelle14" ref="B13:F15" totalsRowShown="0" tableBorderDxfId="5">
   <autoFilter ref="B13:F15" xr:uid="{B264D01E-B1C5-44AC-A123-09E78C0A1D3C}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{35CAF910-5E11-4C98-BDCB-833CA7FD7C95}" name=" "/>
+    <tableColumn id="1" xr3:uid="{35CAF910-5E11-4C98-BDCB-833CA7FD7C95}" name=" " dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{71459494-1BA9-4A53-9244-FF1A5ADDCF75}" name="mid"/>
     <tableColumn id="3" xr3:uid="{44814302-0FAB-4B5B-9D64-6AFE4783B793}" name="player"/>
     <tableColumn id="4" xr3:uid="{F8AB16FD-080F-489A-9596-AF0E16856803}" name="item"/>
@@ -1154,10 +1308,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC29E10A-9C08-4A05-9086-C9A760B6125F}" name="Tabelle2" displayName="Tabelle2" ref="G3:H5" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <autoFilter ref="G3:H5" xr:uid="{454A1DA6-4CBA-4EE8-9389-936CF1CDD9C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC29E10A-9C08-4A05-9086-C9A760B6125F}" name="Tabelle2" displayName="Tabelle2" ref="L24:M26" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+  <autoFilter ref="L24:M26" xr:uid="{454A1DA6-4CBA-4EE8-9389-936CF1CDD9C1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{239B428F-5914-4616-BB28-ACE39A22434A}" name=" " dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{239B428F-5914-4616-BB28-ACE39A22434A}" name=" " dataDxfId="28"/>
     <tableColumn id="2" xr3:uid="{907C80F7-F928-48C1-B45D-8B7F2BD81756}" name="name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1165,10 +1319,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7C718E60-F6FD-436B-A6CB-DA9764FFB495}" name="Tabelle3" displayName="Tabelle3" ref="F18:J20" totalsRowShown="0" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7C718E60-F6FD-436B-A6CB-DA9764FFB495}" name="Tabelle3" displayName="Tabelle3" ref="F18:J20" totalsRowShown="0" tableBorderDxfId="27">
   <autoFilter ref="F18:J20" xr:uid="{BAA7DE8C-DD5A-4893-B04B-F30191F23A0B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{44C27546-60CC-4084-8DA7-938121BD4DD8}" name=" " dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{44C27546-60CC-4084-8DA7-938121BD4DD8}" name=" " dataDxfId="26"/>
     <tableColumn id="2" xr3:uid="{F875BBA2-5C66-4170-A8BA-302DED26D730}" name="mid"/>
     <tableColumn id="3" xr3:uid="{B1CBFB62-9386-4E51-BA90-66DF49A5C99C}" name="player"/>
     <tableColumn id="5" xr3:uid="{8064CD73-A5FF-4E2A-94B3-03654FA70CCF}" name="startrole"/>
@@ -1179,10 +1333,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{822FCC4F-55FE-41D3-B688-A3BC9AB95087}" name="Tabelle4" displayName="Tabelle4" ref="J3:N5" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{822FCC4F-55FE-41D3-B688-A3BC9AB95087}" name="Tabelle4" displayName="Tabelle4" ref="J3:N5" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="J3:N5" xr:uid="{F52E8E40-021E-4471-BC10-A9FF1FC8BA38}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5A1BBBC7-2810-44CB-B915-737D559B2C6D}" name=" " dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{5A1BBBC7-2810-44CB-B915-737D559B2C6D}" name=" " dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{75A0585B-E744-4BCE-9B14-593A7F63D81D}" name="name"/>
     <tableColumn id="3" xr3:uid="{0C542851-5D2F-4808-AFF8-3C2F0C30C757}" name="team"/>
     <tableColumn id="5" xr3:uid="{E1976BC6-4987-4D27-A165-640DCAC50A88}" name="superteam"/>
@@ -1196,7 +1350,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{357D6CAA-DF33-46C1-8889-58556704D715}" name="Tabelle5" displayName="Tabelle5" ref="H8:P10" totalsRowShown="0">
   <autoFilter ref="H8:P10" xr:uid="{32C5A8BE-07D8-4186-A1ED-263E5296B241}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0CE5F855-0B92-46E6-921D-AB0B2AC4DB13}" name=" " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0CE5F855-0B92-46E6-921D-AB0B2AC4DB13}" name=" " dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{A3F198A1-4906-4DB2-A4FC-D49EAEF17788}" name="mid"/>
     <tableColumn id="3" xr3:uid="{1F3F8CE0-77E8-449C-85EA-DFB6C4FC4937}" name="player"/>
     <tableColumn id="4" xr3:uid="{7A6DF6C9-10C2-4CB8-A498-83737D30FD4B}" name="vktrole"/>
@@ -1214,7 +1368,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2FF55995-BED1-4ADB-8024-4F3E431A361D}" name="Tabelle57" displayName="Tabelle57" ref="H13:Q15" totalsRowShown="0">
   <autoFilter ref="H13:Q15" xr:uid="{401E65C2-71AC-4B06-B98F-F12946593E95}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{A71BEE10-E42F-432F-981C-A4CE4BA19270}" name=" " dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{A71BEE10-E42F-432F-981C-A4CE4BA19270}" name=" " dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{0418B8D0-A27E-45B4-95A3-7A28A7873426}" name="mid"/>
     <tableColumn id="3" xr3:uid="{57C7490B-1122-431F-83F9-91FE827D5B21}" name="player"/>
     <tableColumn id="4" xr3:uid="{3C2AB111-3F7D-4D50-9026-C3030824B528}" name="vktrole"/>
@@ -1241,10 +1395,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C2022558-BCF4-4A20-A751-B2D365242E58}" name="Tabelle9" displayName="Tabelle9" ref="B18:D20" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C2022558-BCF4-4A20-A751-B2D365242E58}" name="Tabelle9" displayName="Tabelle9" ref="B18:D20" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="B18:D20" xr:uid="{C2022558-BCF4-4A20-A751-B2D365242E58}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{CF878C07-E058-4CC5-B0B0-D4A3103C0C4E}" name=" " dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{CF878C07-E058-4CC5-B0B0-D4A3103C0C4E}" name=" " dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{A74A4B78-31DD-4C7D-95C0-7D427DEA6813}" name="mid"/>
     <tableColumn id="3" xr3:uid="{41CA0520-4406-4BF2-891F-364ED422B165}" name="team"/>
   </tableColumns>
@@ -1253,14 +1407,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EB9ED773-AC33-429C-A78F-BDB6B255A40A}" name="Tabelle11" displayName="Tabelle11" ref="B8:F10" totalsRowShown="0" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EB9ED773-AC33-429C-A78F-BDB6B255A40A}" name="Tabelle11" displayName="Tabelle11" ref="B8:F10" totalsRowShown="0" tableBorderDxfId="8">
   <autoFilter ref="B8:F10" xr:uid="{EB9ED773-AC33-429C-A78F-BDB6B255A40A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FE18D11D-1881-4A20-81B1-CE46DB24D346}" name=" "/>
+    <tableColumn id="1" xr3:uid="{FE18D11D-1881-4A20-81B1-CE46DB24D346}" name=" " dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{BF946692-53EE-4E40-94C7-D9CAD1117515}" name="mid"/>
     <tableColumn id="3" xr3:uid="{08B630E2-F9B0-4E9C-A159-ECD4C24858E8}" name="player"/>
-    <tableColumn id="4" xr3:uid="{579BCD9B-7012-4A04-8008-E15E0C63293F}" name="causee"/>
-    <tableColumn id="5" xr3:uid="{75098097-761B-4423-8FDB-9C45E9EEF3BC}" name="reason"/>
+    <tableColumn id="4" xr3:uid="{579BCD9B-7012-4A04-8008-E15E0C63293F}" name="time"/>
+    <tableColumn id="5" xr3:uid="{75098097-761B-4423-8FDB-9C45E9EEF3BC}" name="  "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1566,10 +1720,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Q25"/>
+  <dimension ref="B1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="L20" sqref="L19:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,27 +1745,24 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
-        <v>33</v>
+      <c r="B2" s="27" t="s">
+        <v>66</v>
       </c>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
-      <c r="E2" s="27"/>
-      <c r="G2" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="27"/>
-      <c r="J2" s="26" t="s">
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
+      <c r="J2" s="27" t="s">
         <v>11</v>
       </c>
       <c r="K2" s="28"/>
       <c r="L2" s="28"/>
       <c r="M2" s="28"/>
-      <c r="N2" s="27"/>
-      <c r="P2" s="26" t="s">
+      <c r="N2" s="29"/>
+      <c r="P2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="27"/>
+      <c r="Q2" s="29"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -1623,34 +1774,31 @@
       <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="F3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="K3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="L3" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q3" s="17" t="s">
+      <c r="Q3" s="16" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1662,33 +1810,30 @@
         <v>26</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>34</v>
+      <c r="F4" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="P4" s="16" t="s">
+      <c r="K4" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="15" t="s">
         <v>3</v>
       </c>
       <c r="Q4" s="1" t="s">
@@ -1705,48 +1850,43 @@
       <c r="D5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="33">
         <v>44342</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>7</v>
-      </c>
+      <c r="F5" s="19"/>
       <c r="J5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="K5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="N5" s="20" t="s">
+      <c r="N5" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="P5" s="18" t="s">
+      <c r="P5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q5" s="19" t="s">
+      <c r="Q5" s="18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="26" t="s">
-        <v>50</v>
+      <c r="B7" s="27" t="s">
+        <v>49</v>
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
-      <c r="F7" s="27"/>
-      <c r="H7" s="26" t="s">
-        <v>49</v>
+      <c r="F7" s="29"/>
+      <c r="H7" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
@@ -1755,7 +1895,7 @@
       <c r="M7" s="28"/>
       <c r="N7" s="28"/>
       <c r="O7" s="28"/>
-      <c r="P7" s="27"/>
+      <c r="P7" s="29"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
@@ -1768,12 +1908,12 @@
         <v>10</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="6" t="s">
@@ -1786,38 +1926,36 @@
         <v>21</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P8" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="H9" s="12" t="s">
         <v>3</v>
       </c>
       <c r="I9" s="6" t="s">
@@ -1827,7 +1965,7 @@
         <v>12</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>25</v>
@@ -1836,17 +1974,17 @@
         <v>12</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P9" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="6">
@@ -1855,7 +1993,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="13" t="s">
         <v>4</v>
       </c>
       <c r="I10" s="9">
@@ -1865,34 +2003,34 @@
         <v>17</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N10" s="9" t="s">
         <v>14</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="P10" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="P10" s="19" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="26" t="s">
-        <v>52</v>
+      <c r="B12" s="27" t="s">
+        <v>51</v>
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
       <c r="E12" s="28"/>
-      <c r="F12" s="27"/>
-      <c r="H12" s="26" t="s">
+      <c r="F12" s="29"/>
+      <c r="H12" s="27" t="s">
         <v>19</v>
       </c>
       <c r="I12" s="28"/>
@@ -1903,7 +2041,7 @@
       <c r="N12" s="28"/>
       <c r="O12" s="28"/>
       <c r="P12" s="28"/>
-      <c r="Q12" s="27"/>
+      <c r="Q12" s="29"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
@@ -1916,7 +2054,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>16</v>
@@ -1934,16 +2072,16 @@
         <v>21</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>15</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P13" s="6" t="s">
         <v>20</v>
@@ -1953,17 +2091,17 @@
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>29</v>
@@ -1978,7 +2116,7 @@
         <v>12</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>25</v>
@@ -1987,10 +2125,10 @@
         <v>12</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>26</v>
@@ -2000,7 +2138,7 @@
       </c>
     </row>
     <row r="15" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="6">
@@ -2019,116 +2157,116 @@
         <v>17</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L15" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="M15" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="M15" s="9" t="s">
-        <v>62</v>
-      </c>
       <c r="N15" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P15" s="9">
         <v>10</v>
       </c>
-      <c r="Q15" s="20" t="s">
-        <v>63</v>
+      <c r="Q15" s="19" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34"/>
-      <c r="F17" s="26" t="s">
+      <c r="B17" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
+      <c r="F17" s="27" t="s">
         <v>8</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
-      <c r="J17" s="27"/>
-      <c r="L17" s="26" t="s">
-        <v>47</v>
+      <c r="J17" s="29"/>
+      <c r="L17" s="27" t="s">
+        <v>46</v>
       </c>
       <c r="M17" s="28"/>
       <c r="N17" s="28"/>
-      <c r="O17" s="27"/>
+      <c r="O17" s="29"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="11" t="s">
         <v>0</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>10</v>
       </c>
       <c r="I18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J18" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L18" s="29" t="s">
+      <c r="L18" s="25" t="s">
         <v>9</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>0</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>3</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L19" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19" s="15" t="s">
         <v>3</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N19" s="6" t="s">
         <v>12</v>
@@ -2138,31 +2276,31 @@
       </c>
     </row>
     <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="18">
         <v>1</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="14" t="s">
+      <c r="D20" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="14">
         <v>1</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>13</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J20" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="L20" s="30" t="s">
+      <c r="L20" s="15" t="s">
         <v>4</v>
       </c>
       <c r="M20" s="9">
@@ -2171,24 +2309,25 @@
       <c r="N20" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="O20" s="20" t="s">
-        <v>66</v>
+      <c r="O20" s="19" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="26" t="s">
-        <v>51</v>
+    <row r="22" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="27" t="s">
+        <v>50</v>
       </c>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
-      <c r="H22" s="27"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="29"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="25" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -2198,24 +2337,31 @@
         <v>10</v>
       </c>
       <c r="E23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="G23" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="I23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L23" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="M23" s="29"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>12</v>
@@ -2224,42 +2370,66 @@
         <v>12</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>29</v>
       </c>
+      <c r="I24" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M24" s="16" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
+    <row r="25" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="9">
         <v>1</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="19"/>
+      <c r="L25" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L26" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="M26" s="18" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B22:I22"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="H12:Q12"/>
     <mergeCell ref="L17:O17"/>
     <mergeCell ref="H7:P7"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:N2"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="63" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
small fix in logparser, reparsed log, updated db schema while implementing parsing
</commit_message>
<xml_diff>
--- a/database schema.xlsx
+++ b/database schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\git\TTTStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2831CEE-BCEE-4B7E-9277-4DA2FDA777D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65EB201-9D75-4440-8C99-11D898B427F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{999ED5BF-1C97-4366-969E-3A684A32F4E0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="73">
   <si>
     <t>mid</t>
   </si>
@@ -243,6 +243,15 @@
   </si>
   <si>
     <t>crole</t>
+  </si>
+  <si>
+    <t>teamdmg</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>teamkill</t>
   </si>
 </sst>
 </file>
@@ -277,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,6 +308,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -498,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -526,13 +541,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -544,12 +560,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -587,6 +630,22 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -623,6 +682,19 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -659,6 +731,19 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -695,69 +780,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <left style="medium">
           <color indexed="64"/>
@@ -808,57 +830,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
         <right style="medium">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -973,6 +954,147 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1011,79 +1133,11 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1123,10 +1177,57 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1151,72 +1252,6 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1250,10 +1285,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E1C6EE2-18C0-43EE-8AD5-4B7F873C290E}" name="Tabelle1" displayName="Tabelle1" ref="B3:F5" totalsRowShown="0" headerRowDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E1C6EE2-18C0-43EE-8AD5-4B7F873C290E}" name="Tabelle1" displayName="Tabelle1" ref="B3:F5" totalsRowShown="0" headerRowDxfId="35">
   <autoFilter ref="B3:F5" xr:uid="{52BD7EF9-37E0-4ECA-A811-5669E3CF00AA}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{28B5F67C-42FE-4CC0-9F2B-12521EDBA32C}" name=" " dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{28B5F67C-42FE-4CC0-9F2B-12521EDBA32C}" name=" " dataDxfId="34"/>
     <tableColumn id="2" xr3:uid="{F6E5BE1F-762D-4412-BB71-B6D6EE94D6C5}" name="mid"/>
     <tableColumn id="3" xr3:uid="{820B8EBD-28D3-4E1A-8BDA-917DE40A720A}" name="map"/>
     <tableColumn id="5" xr3:uid="{4DD32033-EEC8-40B7-B044-AC965EEDD732}" name="date"/>
@@ -1264,27 +1299,27 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{74C74E02-A02B-41C4-BADC-5A81D4707866}" name="Tabelle12" displayName="Tabelle12" ref="B23:I25" totalsRowShown="0" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{74C74E02-A02B-41C4-BADC-5A81D4707866}" name="Tabelle12" displayName="Tabelle12" ref="B23:I25" totalsRowShown="0" tableBorderDxfId="9">
   <autoFilter ref="B23:I25" xr:uid="{74C74E02-A02B-41C4-BADC-5A81D4707866}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{2F3D3C50-1B81-4C2A-AC27-145F73A517B4}" name=" " dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{2F3D3C50-1B81-4C2A-AC27-145F73A517B4}" name=" " dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{BFBE01E6-D2F9-4FEC-98E5-6FD7BFEE4A15}" name="mid"/>
     <tableColumn id="3" xr3:uid="{D252F81D-FEAA-49CD-8D7B-FD6F074A08A2}" name="player"/>
-    <tableColumn id="4" xr3:uid="{8731F0A4-8107-43FD-9F22-FA4CF46A2C14}" name="causee"/>
+    <tableColumn id="4" xr3:uid="{8731F0A4-8107-43FD-9F22-FA4CF46A2C14}" name="causee" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{6DFDAEE0-AEC1-45E5-9E8B-AA9DD78D8CBF}" name="fromrole"/>
     <tableColumn id="6" xr3:uid="{398BB72D-970E-4531-9612-81F2C3C547E0}" name="torole"/>
     <tableColumn id="7" xr3:uid="{D216005C-1E93-4949-AA8B-09D52C12C24A}" name="time"/>
-    <tableColumn id="8" xr3:uid="{4F52CAD3-EA0D-4037-AE32-B99C8E0B1EA7}" name="crole"/>
+    <tableColumn id="8" xr3:uid="{4F52CAD3-EA0D-4037-AE32-B99C8E0B1EA7}" name="crole" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{C6772C9E-B684-4967-B1B0-2F5D7E931EAD}" name="Tabelle13" displayName="Tabelle13" ref="L18:O20" totalsRowShown="0" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{C6772C9E-B684-4967-B1B0-2F5D7E931EAD}" name="Tabelle13" displayName="Tabelle13" ref="L18:O20" totalsRowShown="0" tableBorderDxfId="7">
   <autoFilter ref="L18:O20" xr:uid="{C6772C9E-B684-4967-B1B0-2F5D7E931EAD}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{11ADBF08-FA1E-4F08-91A9-89729F535445}" name=" " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{11ADBF08-FA1E-4F08-91A9-89729F535445}" name=" " dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{754DA27A-3AA8-4E40-949D-9264EF980EDD}" name="mid"/>
     <tableColumn id="3" xr3:uid="{6B3182E9-F4BF-4CA5-B320-DB44C252EF32}" name="first"/>
     <tableColumn id="4" xr3:uid="{B089E9C9-3B3E-4AAF-9B5A-7F3033018EBB}" name="second"/>
@@ -1294,24 +1329,25 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B264D01E-B1C5-44AC-A123-09E78C0A1D3C}" name="Tabelle14" displayName="Tabelle14" ref="B13:F15" totalsRowShown="0" tableBorderDxfId="5">
-  <autoFilter ref="B13:F15" xr:uid="{B264D01E-B1C5-44AC-A123-09E78C0A1D3C}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{35CAF910-5E11-4C98-BDCB-833CA7FD7C95}" name=" " dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B264D01E-B1C5-44AC-A123-09E78C0A1D3C}" name="Tabelle14" displayName="Tabelle14" ref="B13:G15" totalsRowShown="0" tableBorderDxfId="5">
+  <autoFilter ref="B13:G15" xr:uid="{B264D01E-B1C5-44AC-A123-09E78C0A1D3C}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{35CAF910-5E11-4C98-BDCB-833CA7FD7C95}" name=" " dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{71459494-1BA9-4A53-9244-FF1A5ADDCF75}" name="mid"/>
     <tableColumn id="3" xr3:uid="{44814302-0FAB-4B5B-9D64-6AFE4783B793}" name="player"/>
     <tableColumn id="4" xr3:uid="{F8AB16FD-080F-489A-9596-AF0E16856803}" name="item"/>
     <tableColumn id="5" xr3:uid="{0AFE03ED-82E8-4D41-87C5-80B654E288B0}" name="time"/>
+    <tableColumn id="6" xr3:uid="{B0212047-98D8-4874-BF17-4BB1F05FEEBE}" name="role"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC29E10A-9C08-4A05-9086-C9A760B6125F}" name="Tabelle2" displayName="Tabelle2" ref="L24:M26" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC29E10A-9C08-4A05-9086-C9A760B6125F}" name="Tabelle2" displayName="Tabelle2" ref="L24:M26" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="L24:M26" xr:uid="{454A1DA6-4CBA-4EE8-9389-936CF1CDD9C1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{239B428F-5914-4616-BB28-ACE39A22434A}" name=" " dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{239B428F-5914-4616-BB28-ACE39A22434A}" name=" " dataDxfId="29"/>
     <tableColumn id="2" xr3:uid="{907C80F7-F928-48C1-B45D-8B7F2BD81756}" name="name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1319,10 +1355,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7C718E60-F6FD-436B-A6CB-DA9764FFB495}" name="Tabelle3" displayName="Tabelle3" ref="F18:J20" totalsRowShown="0" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7C718E60-F6FD-436B-A6CB-DA9764FFB495}" name="Tabelle3" displayName="Tabelle3" ref="F18:J20" totalsRowShown="0" tableBorderDxfId="28">
   <autoFilter ref="F18:J20" xr:uid="{BAA7DE8C-DD5A-4893-B04B-F30191F23A0B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{44C27546-60CC-4084-8DA7-938121BD4DD8}" name=" " dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{44C27546-60CC-4084-8DA7-938121BD4DD8}" name=" " dataDxfId="27"/>
     <tableColumn id="2" xr3:uid="{F875BBA2-5C66-4170-A8BA-302DED26D730}" name="mid"/>
     <tableColumn id="3" xr3:uid="{B1CBFB62-9386-4E51-BA90-66DF49A5C99C}" name="player"/>
     <tableColumn id="5" xr3:uid="{8064CD73-A5FF-4E2A-94B3-03654FA70CCF}" name="startrole"/>
@@ -1333,10 +1369,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{822FCC4F-55FE-41D3-B688-A3BC9AB95087}" name="Tabelle4" displayName="Tabelle4" ref="J3:N5" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{822FCC4F-55FE-41D3-B688-A3BC9AB95087}" name="Tabelle4" displayName="Tabelle4" ref="J3:N5" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="J3:N5" xr:uid="{F52E8E40-021E-4471-BC10-A9FF1FC8BA38}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5A1BBBC7-2810-44CB-B915-737D559B2C6D}" name=" " dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{5A1BBBC7-2810-44CB-B915-737D559B2C6D}" name=" " dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{75A0585B-E744-4BCE-9B14-593A7F63D81D}" name="name"/>
     <tableColumn id="3" xr3:uid="{0C542851-5D2F-4808-AFF8-3C2F0C30C757}" name="team"/>
     <tableColumn id="5" xr3:uid="{E1976BC6-4987-4D27-A165-640DCAC50A88}" name="superteam"/>
@@ -1347,10 +1383,10 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{357D6CAA-DF33-46C1-8889-58556704D715}" name="Tabelle5" displayName="Tabelle5" ref="H8:P10" totalsRowShown="0">
-  <autoFilter ref="H8:P10" xr:uid="{32C5A8BE-07D8-4186-A1ED-263E5296B241}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0CE5F855-0B92-46E6-921D-AB0B2AC4DB13}" name=" " dataDxfId="20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{357D6CAA-DF33-46C1-8889-58556704D715}" name="Tabelle5" displayName="Tabelle5" ref="H8:Q10" totalsRowShown="0">
+  <autoFilter ref="H8:Q10" xr:uid="{32C5A8BE-07D8-4186-A1ED-263E5296B241}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{0CE5F855-0B92-46E6-921D-AB0B2AC4DB13}" name=" " dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{A3F198A1-4906-4DB2-A4FC-D49EAEF17788}" name="mid"/>
     <tableColumn id="3" xr3:uid="{1F3F8CE0-77E8-449C-85EA-DFB6C4FC4937}" name="player"/>
     <tableColumn id="4" xr3:uid="{7A6DF6C9-10C2-4CB8-A498-83737D30FD4B}" name="vktrole"/>
@@ -1359,16 +1395,17 @@
     <tableColumn id="9" xr3:uid="{4BEC3DB9-57AF-4B72-BB20-2A526C6A0ED9}" name="atkrole"/>
     <tableColumn id="8" xr3:uid="{6B455A4E-61C8-4F7F-B6A4-252B2CB182F4}" name="weapon"/>
     <tableColumn id="7" xr3:uid="{6A5B3ED8-A41F-46F2-9BFB-DB1F20464E8A}" name="time"/>
+    <tableColumn id="10" xr3:uid="{ADAD4C65-7A3A-4EBB-9744-60F46B7CD12B}" name="teamkill"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2FF55995-BED1-4ADB-8024-4F3E431A361D}" name="Tabelle57" displayName="Tabelle57" ref="H13:Q15" totalsRowShown="0">
-  <autoFilter ref="H13:Q15" xr:uid="{401E65C2-71AC-4B06-B98F-F12946593E95}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{A71BEE10-E42F-432F-981C-A4CE4BA19270}" name=" " dataDxfId="19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2FF55995-BED1-4ADB-8024-4F3E431A361D}" name="Tabelle57" displayName="Tabelle57" ref="I13:S15" totalsRowShown="0">
+  <autoFilter ref="I13:S15" xr:uid="{401E65C2-71AC-4B06-B98F-F12946593E95}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{A71BEE10-E42F-432F-981C-A4CE4BA19270}" name=" " dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{0418B8D0-A27E-45B4-95A3-7A28A7873426}" name="mid"/>
     <tableColumn id="3" xr3:uid="{57C7490B-1122-431F-83F9-91FE827D5B21}" name="player"/>
     <tableColumn id="4" xr3:uid="{3C2AB111-3F7D-4D50-9026-C3030824B528}" name="vktrole"/>
@@ -1378,16 +1415,17 @@
     <tableColumn id="10" xr3:uid="{FF555FE5-B1A8-402F-96B8-1915C15BDF86}" name="weapon"/>
     <tableColumn id="9" xr3:uid="{6EA4795D-0357-4C1B-8960-A01B91FE8EBE}" name="damage"/>
     <tableColumn id="8" xr3:uid="{810AC511-47D1-47A2-80EB-E6D1478028FC}" name="time"/>
+    <tableColumn id="11" xr3:uid="{8253BF86-4C41-4764-AD85-EE92CF2D357A}" name="teamdmg"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C1563867-70DF-4091-83F3-B3B42F5161BB}" name="Tabelle28" displayName="Tabelle28" ref="P3:Q5" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C1563867-70DF-4091-83F3-B3B42F5161BB}" name="Tabelle28" displayName="Tabelle28" ref="P3:Q5" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <autoFilter ref="P3:Q5" xr:uid="{11560C94-C78A-4C22-B229-87B96A147E98}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{847738E0-6F98-4A70-A98A-2FB31829D010}" name=" " dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{847738E0-6F98-4A70-A98A-2FB31829D010}" name=" " dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{066970CC-1FA8-43B1-9EC6-AE9D55C6A3F3}" name="filename"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1395,10 +1433,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C2022558-BCF4-4A20-A751-B2D365242E58}" name="Tabelle9" displayName="Tabelle9" ref="B18:D20" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C2022558-BCF4-4A20-A751-B2D365242E58}" name="Tabelle9" displayName="Tabelle9" ref="B18:D20" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="B18:D20" xr:uid="{C2022558-BCF4-4A20-A751-B2D365242E58}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{CF878C07-E058-4CC5-B0B0-D4A3103C0C4E}" name=" " dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{CF878C07-E058-4CC5-B0B0-D4A3103C0C4E}" name=" " dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{A74A4B78-31DD-4C7D-95C0-7D427DEA6813}" name="mid"/>
     <tableColumn id="3" xr3:uid="{41CA0520-4406-4BF2-891F-364ED422B165}" name="team"/>
   </tableColumns>
@@ -1407,10 +1445,10 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EB9ED773-AC33-429C-A78F-BDB6B255A40A}" name="Tabelle11" displayName="Tabelle11" ref="B8:F10" totalsRowShown="0" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EB9ED773-AC33-429C-A78F-BDB6B255A40A}" name="Tabelle11" displayName="Tabelle11" ref="B8:F10" totalsRowShown="0" tableBorderDxfId="11">
   <autoFilter ref="B8:F10" xr:uid="{EB9ED773-AC33-429C-A78F-BDB6B255A40A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FE18D11D-1881-4A20-81B1-CE46DB24D346}" name=" " dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{FE18D11D-1881-4A20-81B1-CE46DB24D346}" name=" " dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{BF946692-53EE-4E40-94C7-D9CAD1117515}" name="mid"/>
     <tableColumn id="3" xr3:uid="{08B630E2-F9B0-4E9C-A159-ECD4C24858E8}" name="player"/>
     <tableColumn id="4" xr3:uid="{579BCD9B-7012-4A04-8008-E15E0C63293F}" name="time"/>
@@ -1720,10 +1758,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Q26"/>
+  <dimension ref="B1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L20" sqref="L19:L20"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1743,28 +1781,28 @@
     <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+    <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="F2" s="29"/>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
       <c r="N2" s="29"/>
-      <c r="P2" s="27" t="s">
+      <c r="P2" s="28" t="s">
         <v>30</v>
       </c>
       <c r="Q2" s="29"/>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1802,7 +1840,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1840,7 +1878,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
@@ -1850,7 +1888,7 @@
       <c r="D5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="27">
         <v>44342</v>
       </c>
       <c r="F5" s="19"/>
@@ -1876,28 +1914,29 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="27" t="s">
+    <row r="6" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
       <c r="F7" s="29"/>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="29"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="29"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
@@ -1937,11 +1976,14 @@
       <c r="O8" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="P8" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="Q8" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>3</v>
       </c>
@@ -1979,11 +2021,14 @@
       <c r="O9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P9" s="7" t="s">
+      <c r="P9" s="6" t="s">
         <v>29</v>
       </c>
+      <c r="Q9" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="10" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
         <v>4</v>
       </c>
@@ -2017,34 +2062,37 @@
       <c r="O10" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="P10" s="19" t="s">
+      <c r="P10" s="9" t="s">
         <v>18</v>
       </c>
+      <c r="Q10" s="19"/>
     </row>
-    <row r="11" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="27" t="s">
+    <row r="11" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
-      <c r="H12" s="27" t="s">
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="29"/>
+      <c r="I12" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="29"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="29"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="25" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -2059,39 +2107,45 @@
       <c r="F13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="G13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="J13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="K13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="L13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="M13" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="N13" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="O13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O13" s="6" t="s">
+      <c r="P13" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="P13" s="6" t="s">
+      <c r="Q13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q13" s="7" t="s">
+      <c r="R13" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="S13" s="7" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -2106,64 +2160,68 @@
       <c r="F14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="G14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="J14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="K14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="L14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="M14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="N14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N14" s="6" t="s">
+      <c r="O14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O14" s="6" t="s">
+      <c r="P14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P14" s="6" t="s">
+      <c r="Q14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="Q14" s="7" t="s">
+      <c r="R14" s="6" t="s">
         <v>29</v>
       </c>
+      <c r="S14" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="15" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="15" t="s">
+    <row r="15" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="H15" s="8" t="s">
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="19"/>
+      <c r="I15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="9">
+      <c r="J15" s="9">
         <v>1</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="K15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="L15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="M15" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="M15" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="N15" s="9" t="s">
         <v>61</v>
@@ -2171,32 +2229,36 @@
       <c r="O15" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="P15" s="9">
+      <c r="P15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q15" s="9">
         <v>10</v>
       </c>
-      <c r="Q15" s="19" t="s">
+      <c r="R15" s="9" t="s">
         <v>62</v>
       </c>
+      <c r="S15" s="19"/>
     </row>
-    <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
-      <c r="F17" s="27" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="33"/>
+      <c r="F17" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
       <c r="J17" s="29"/>
-      <c r="L17" s="27" t="s">
+      <c r="L17" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
       <c r="O17" s="29"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
@@ -2315,15 +2377,15 @@
     </row>
     <row r="21" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
       <c r="I22" s="29"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
@@ -2336,7 +2398,7 @@
       <c r="D23" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="34" t="s">
         <v>54</v>
       </c>
       <c r="F23" s="6" t="s">
@@ -2348,10 +2410,10 @@
       <c r="H23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="I23" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="L23" s="27" t="s">
+      <c r="L23" s="28" t="s">
         <v>10</v>
       </c>
       <c r="M23" s="29"/>
@@ -2366,7 +2428,7 @@
       <c r="D24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="34" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -2378,7 +2440,7 @@
       <c r="H24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I24" s="36" t="s">
         <v>40</v>
       </c>
       <c r="L24" s="16" t="s">
@@ -2396,11 +2458,11 @@
         <v>1</v>
       </c>
       <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
+      <c r="E25" s="35"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
-      <c r="I25" s="19"/>
+      <c r="I25" s="37"/>
       <c r="L25" s="15" t="s">
         <v>3</v>
       </c>
@@ -2426,10 +2488,10 @@
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="H12:Q12"/>
     <mergeCell ref="L17:O17"/>
-    <mergeCell ref="H7:P7"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="H7:Q7"/>
+    <mergeCell ref="I12:S12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="63" orientation="landscape" r:id="rId1"/>

</xml_diff>